<commit_message>
Initializating the project for me
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vicen\git\algorithmicsGarciaDiazVicenteUO42478\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD47017-13A3-40B4-A991-1C202C3B8F53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4B75DDF2-FAFD-41DF-BD15-78FA89FEE8DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="20790" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Marks" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -159,9 +155,6 @@
     <t>Please, don't change this file after you indicate your name</t>
   </si>
   <si>
-    <t>García Díaz, Vicente</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Total maximum possible </t>
     </r>
@@ -206,6 +199,9 @@
   </si>
   <si>
     <t>Each session will be graded with a score between 0 and 10</t>
+  </si>
+  <si>
+    <t>Gómez Menéndez, Laura</t>
   </si>
 </sst>
 </file>
@@ -874,7 +870,7 @@
   <dimension ref="A1:J136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -901,25 +897,25 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>2</v>
@@ -930,7 +926,7 @@
     </row>
     <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1030,12 +1026,12 @@
     </row>
     <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>